<commit_message>
charts inserted, typos fixed
</commit_message>
<xml_diff>
--- a/Documents/CS320_Excel_Works.xlsx
+++ b/Documents/CS320_Excel_Works.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metinkaraca/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90534\OneDrive\Desktop\Courses\CS320\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EFE3BB-EB12-1343-9535-D2BCA8E51F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5878289-F197-47A9-8664-A5D6448FADBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{989A74A3-1140-104B-93D7-3DED2FDBFEEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{989A74A3-1140-104B-93D7-3DED2FDBFEEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,10 +338,6 @@
     <t>Instead of campus's internet, mobile hotspot will be used.</t>
   </si>
   <si>
-    <t>In case of not integrating  database, CSV will be used to
-to save the datas.</t>
-  </si>
-  <si>
     <t>Software needs exact 3 computers. If something happens to computers, computers will be substituted.</t>
   </si>
   <si>
@@ -373,6 +369,9 @@
   </si>
   <si>
     <t>Failure to meet at arranged schedule; failure to fix reported problems.</t>
+  </si>
+  <si>
+    <t>In case of not integrating  database, CSV will be used to save the datas.</t>
   </si>
 </sst>
 </file>
@@ -983,26 +982,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,33 +1323,33 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="56.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
     <col min="10" max="10" width="71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="D5" s="72" t="s">
+    <row r="5" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="I5" s="72" t="s">
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="I5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="72"/>
+      <c r="J5" s="78"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="3:17" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="3:17" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:17" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="D8" s="39" t="s">
         <v>29</v>
@@ -1412,7 +1411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="38" t="s">
         <v>35</v>
@@ -1444,7 +1443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="3:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
       <c r="D10" s="40" t="s">
         <v>32</v>
@@ -1476,7 +1475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="3:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
         <v>36</v>
@@ -1508,7 +1507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="3" t="s">
         <v>39</v>
@@ -1536,7 +1535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="46" t="s">
         <v>38</v>
@@ -1564,7 +1563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
       <c r="D14" s="46" t="s">
         <v>38</v>
@@ -1590,7 +1589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="46" t="s">
         <v>38</v>
@@ -1615,7 +1614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="46" t="s">
         <v>38</v>
@@ -1640,7 +1639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="46" t="s">
         <v>38</v>
@@ -1665,7 +1664,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="D18" s="46" t="s">
         <v>38</v>
@@ -1688,7 +1687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="D19" s="46" t="s">
         <v>38</v>
@@ -1707,7 +1706,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="46" t="s">
         <v>38</v>
@@ -1726,7 +1725,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="46" t="s">
         <v>38</v>
@@ -1745,11 +1744,11 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
     </row>
-    <row r="27" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="3:15" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="34" t="s">
         <v>54</v>
       </c>
@@ -1769,7 +1768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="3:15" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:15" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D29" s="44" t="s">
         <v>46</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="45" t="s">
         <v>43</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="3:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="47" t="s">
         <v>47</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="3:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="59" t="s">
         <v>48</v>
       </c>
@@ -1801,11 +1800,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
       <c r="E33" s="14"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="K40" s="1"/>
     </row>
   </sheetData>
@@ -1825,18 +1824,18 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="70"/>
       <c r="E4" s="70"/>
       <c r="F4" s="70"/>
@@ -1845,7 +1844,7 @@
       <c r="I4" s="70"/>
       <c r="J4" s="70"/>
     </row>
-    <row r="5" spans="4:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="68" t="s">
         <v>54</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="4:10" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:10" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D6" s="61" t="s">
         <v>63</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="4:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D7" s="19" t="s">
         <v>64</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="4:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D8" s="64" t="s">
         <v>65</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="4:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D9" s="66" t="s">
         <v>62</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D10" s="25" t="s">
         <v>66</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="4:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D11" s="66" t="s">
         <v>61</v>
       </c>
@@ -2015,103 +2014,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F800A32-87BE-014B-9354-21B52D42D018}">
   <dimension ref="E9:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
     <col min="6" max="6" width="42.5" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="5:6" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="5:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="5:6" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E11" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" spans="5:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E12" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="56"/>
-    </row>
-    <row r="12" spans="5:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="E12" s="45" t="s">
+      <c r="F12" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F13" s="58"/>
+    </row>
+    <row r="14" spans="5:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E14" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="60" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="5:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E13" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="58"/>
-    </row>
-    <row r="14" spans="5:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="E14" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="52"/>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
       <c r="F18" s="53"/>
     </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
       <c r="F19" s="54"/>
     </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20" s="53"/>
     </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="54"/>
     </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
       <c r="F22" s="53"/>
     </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E23" s="9"/>
       <c r="F23" s="52"/>
     </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E24" s="5"/>
       <c r="F24" s="55"/>
     </row>
-    <row r="25" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="5:9" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="5:9" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H26" s="34" t="s">
         <v>0</v>
       </c>
@@ -2119,7 +2118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="5:9" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="H27" s="44" t="s">
         <v>93</v>
       </c>
@@ -2127,62 +2126,62 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="5:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H28" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I28" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="5:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H29" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I29" s="58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="5:9" ht="34" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H30" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="76" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="5:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="I30" s="75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="5:9" x14ac:dyDescent="0.25">
       <c r="H31" s="47" t="s">
         <v>39</v>
       </c>
       <c r="I31" s="58" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="10:12" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="74" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="10:12" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="K33" s="75" t="s">
+      <c r="K33" s="74" t="s">
         <v>1</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="10:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="J34" s="77" t="s">
+    <row r="34" spans="10:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="76" t="s">
         <v>93</v>
       </c>
       <c r="K34" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="78" t="s">
+      <c r="L34" s="77" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J35" s="40" t="s">
         <v>32</v>
       </c>
@@ -2193,8 +2192,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J36" s="73" t="s">
+    <row r="36" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="72" t="s">
         <v>94</v>
       </c>
       <c r="K36" s="24" t="s">
@@ -2204,7 +2203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J37" s="3" t="s">
         <v>39</v>
       </c>
@@ -2215,9 +2214,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J38" s="73" t="s">
-        <v>99</v>
+    <row r="38" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J38" s="72" t="s">
+        <v>98</v>
       </c>
       <c r="K38" s="24" t="s">
         <v>37</v>
@@ -2226,9 +2225,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K39" s="26" t="s">
         <v>33</v>

</xml_diff>